<commit_message>
Screen Cast method added
</commit_message>
<xml_diff>
--- a/Castle/data/amazonSearch.xlsx
+++ b/Castle/data/amazonSearch.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Items</t>
   </si>
@@ -120,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -148,6 +148,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
@@ -653,7 +680,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="37" t="s">
         <v>11</v>
       </c>
     </row>
@@ -661,7 +688,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="38" t="s">
         <v>12</v>
       </c>
     </row>
@@ -669,7 +696,7 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="39" t="s">
         <v>13</v>
       </c>
     </row>
@@ -677,7 +704,7 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="40" t="s">
         <v>19</v>
       </c>
     </row>
@@ -685,7 +712,7 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="41" t="s">
         <v>20</v>
       </c>
     </row>
@@ -693,7 +720,7 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="42" t="s">
         <v>15</v>
       </c>
     </row>
@@ -701,7 +728,7 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="43" t="s">
         <v>16</v>
       </c>
     </row>
@@ -709,7 +736,7 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="44" t="s">
         <v>17</v>
       </c>
     </row>
@@ -717,7 +744,7 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="45" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>